<commit_message>
:bento: update Eldo Meadows times for March to use real data
</commit_message>
<xml_diff>
--- a/resources/references/pretoriareferencedoc.xlsx
+++ b/resources/references/pretoriareferencedoc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Pretoria" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Pretoria!$A$2:$J$380</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Pretoria!$A$2:$J$380</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">Pretoria!$A$2:$J$380</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">Pretoria!$A$2:$J$380</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -119,10 +120,10 @@
     <t xml:space="preserve">jummah_salaah</t>
   </si>
   <si>
-    <t xml:space="preserve">zohr_athan_special</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zohr_salaah_special</t>
+    <t xml:space="preserve">zuhr_athan_special</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zuhr_salaah_special</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -1785,16 +1786,16 @@
   <dimension ref="A2:W378"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X12" activeCellId="0" sqref="X12"/>
+      <selection pane="topLeft" activeCell="T7" activeCellId="0" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>

</xml_diff>